<commit_message>
TEST: Test done on 2022-10-05
</commit_message>
<xml_diff>
--- a/test_scenario.xlsx
+++ b/test_scenario.xlsx
@@ -1420,10 +1420,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F116"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+    <sheetView tabSelected="1" topLeftCell="C97" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="topRight" activeCell="G116" sqref="G116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1433,9 +1435,10 @@
     <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="80.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1454,8 +1457,11 @@
       <c r="F1" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G1" s="1">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1463,7 +1469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1482,8 +1488,11 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1502,8 +1511,11 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1522,8 +1534,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1542,8 +1557,11 @@
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1562,8 +1580,11 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1582,8 +1603,11 @@
       <c r="F8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1602,8 +1626,11 @@
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1622,13 +1649,16 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1647,8 +1677,11 @@
       <c r="F12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1667,8 +1700,11 @@
       <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1687,8 +1723,11 @@
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1707,8 +1746,11 @@
       <c r="F15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1727,8 +1769,11 @@
       <c r="F16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1741,8 +1786,11 @@
       <c r="D17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1755,8 +1803,11 @@
       <c r="D18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1775,8 +1826,11 @@
       <c r="F19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1795,8 +1849,11 @@
       <c r="F20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1815,8 +1872,11 @@
       <c r="F21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1835,13 +1895,16 @@
       <c r="F22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>46</v>
       </c>
@@ -1857,8 +1920,11 @@
       <c r="F24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1877,8 +1943,11 @@
       <c r="F25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1897,13 +1966,16 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>51</v>
       </c>
@@ -1919,8 +1991,11 @@
       <c r="F28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1939,8 +2014,11 @@
       <c r="F29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1959,8 +2037,11 @@
       <c r="F30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1979,8 +2060,11 @@
       <c r="F31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1999,8 +2083,11 @@
       <c r="F32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -2019,8 +2106,11 @@
       <c r="F33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -2039,8 +2129,11 @@
       <c r="F34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>266</v>
       </c>
@@ -2056,8 +2149,11 @@
       <c r="F35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -2065,7 +2161,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>54</v>
       </c>
@@ -2081,8 +2177,11 @@
       <c r="F37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>61</v>
       </c>
@@ -2098,8 +2197,11 @@
       <c r="F38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>63</v>
       </c>
@@ -2115,8 +2217,11 @@
       <c r="F39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
         <v>71</v>
       </c>
@@ -2132,8 +2237,11 @@
       <c r="F40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>56</v>
       </c>
@@ -2149,14 +2257,17 @@
       <c r="F41">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>67</v>
       </c>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
         <v>72</v>
       </c>
@@ -2172,8 +2283,11 @@
       <c r="F44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
         <v>73</v>
       </c>
@@ -2189,8 +2303,11 @@
       <c r="F45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
         <v>75</v>
       </c>
@@ -2206,8 +2323,11 @@
       <c r="F46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
         <v>78</v>
       </c>
@@ -2223,8 +2343,11 @@
       <c r="F47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B48" t="s">
         <v>80</v>
       </c>
@@ -2240,8 +2363,11 @@
       <c r="F48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B49" t="s">
         <v>82</v>
       </c>
@@ -2257,8 +2383,11 @@
       <c r="F49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
         <v>107</v>
       </c>
@@ -2274,8 +2403,11 @@
       <c r="F50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
         <v>273</v>
       </c>
@@ -2291,13 +2423,16 @@
       <c r="F51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
         <v>91</v>
       </c>
@@ -2313,8 +2448,11 @@
       <c r="F53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
         <v>94</v>
       </c>
@@ -2330,8 +2468,11 @@
       <c r="F54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B55" t="s">
         <v>95</v>
       </c>
@@ -2347,8 +2488,11 @@
       <c r="F55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
         <v>97</v>
       </c>
@@ -2364,8 +2508,11 @@
       <c r="F56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
         <v>99</v>
       </c>
@@ -2381,8 +2528,11 @@
       <c r="F57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
         <v>101</v>
       </c>
@@ -2398,8 +2548,11 @@
       <c r="F58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
         <v>103</v>
       </c>
@@ -2415,8 +2568,11 @@
       <c r="F59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
         <v>105</v>
       </c>
@@ -2432,8 +2588,11 @@
       <c r="F60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
         <v>109</v>
       </c>
@@ -2449,8 +2608,11 @@
       <c r="F61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
         <v>110</v>
       </c>
@@ -2466,8 +2628,11 @@
       <c r="F62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
         <v>112</v>
       </c>
@@ -2483,8 +2648,11 @@
       <c r="F63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
         <v>113</v>
       </c>
@@ -2500,8 +2668,11 @@
       <c r="F64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
         <v>115</v>
       </c>
@@ -2517,8 +2688,11 @@
       <c r="F65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
         <v>117</v>
       </c>
@@ -2534,8 +2708,11 @@
       <c r="F66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
         <v>269</v>
       </c>
@@ -2551,8 +2728,11 @@
       <c r="F67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
         <v>275</v>
       </c>
@@ -2568,13 +2748,16 @@
       <c r="F68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
         <v>119</v>
       </c>
@@ -2590,8 +2773,11 @@
       <c r="F70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
         <v>121</v>
       </c>
@@ -2607,8 +2793,11 @@
       <c r="F71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>157</v>
       </c>
@@ -2622,7 +2811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B73" t="s">
         <v>124</v>
       </c>
@@ -2638,8 +2827,11 @@
       <c r="F73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
         <v>128</v>
       </c>
@@ -2655,8 +2847,11 @@
       <c r="F74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
         <v>130</v>
       </c>
@@ -2672,8 +2867,11 @@
       <c r="F75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
         <v>131</v>
       </c>
@@ -2689,8 +2887,11 @@
       <c r="F76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
         <v>134</v>
       </c>
@@ -2706,8 +2907,11 @@
       <c r="F77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
         <v>135</v>
       </c>
@@ -2723,13 +2927,16 @@
       <c r="F78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
         <v>124</v>
       </c>
@@ -2745,8 +2952,11 @@
       <c r="F80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
         <v>125</v>
       </c>
@@ -2762,8 +2972,11 @@
       <c r="F81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B82" t="s">
         <v>126</v>
       </c>
@@ -2779,8 +2992,11 @@
       <c r="F82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B83" t="s">
         <v>127</v>
       </c>
@@ -2796,8 +3012,11 @@
       <c r="F83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B84" t="s">
         <v>254</v>
       </c>
@@ -2813,8 +3032,11 @@
       <c r="F84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B85" t="s">
         <v>256</v>
       </c>
@@ -2830,8 +3052,11 @@
       <c r="F85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B86" t="s">
         <v>258</v>
       </c>
@@ -2847,8 +3072,11 @@
       <c r="F86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B87" t="s">
         <v>261</v>
       </c>
@@ -2864,13 +3092,16 @@
       <c r="F87">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B90" t="s">
         <v>124</v>
       </c>
@@ -2886,8 +3117,11 @@
       <c r="F90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B91" t="s">
         <v>138</v>
       </c>
@@ -2903,8 +3137,11 @@
       <c r="F91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B92" t="s">
         <v>140</v>
       </c>
@@ -2920,8 +3157,11 @@
       <c r="F92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B93" t="s">
         <v>142</v>
       </c>
@@ -2937,8 +3177,11 @@
       <c r="F93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B94" t="s">
         <v>263</v>
       </c>
@@ -2954,13 +3197,16 @@
       <c r="F94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B96" t="s">
         <v>124</v>
       </c>
@@ -2976,8 +3222,11 @@
       <c r="F96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B97" t="s">
         <v>134</v>
       </c>
@@ -2993,8 +3242,11 @@
       <c r="F97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B98" t="s">
         <v>147</v>
       </c>
@@ -3010,8 +3262,11 @@
       <c r="F98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B99" t="s">
         <v>149</v>
       </c>
@@ -3027,8 +3282,11 @@
       <c r="F99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B100" t="s">
         <v>151</v>
       </c>
@@ -3044,8 +3302,11 @@
       <c r="F100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B101" t="s">
         <v>153</v>
       </c>
@@ -3061,8 +3322,11 @@
       <c r="F101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B102" t="s">
         <v>155</v>
       </c>
@@ -3075,13 +3339,16 @@
       <c r="E102">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B105" t="s">
         <v>236</v>
       </c>
@@ -3097,8 +3364,11 @@
       <c r="F105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B106" t="s">
         <v>241</v>
       </c>
@@ -3114,8 +3384,11 @@
       <c r="F106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B107" t="s">
         <v>243</v>
       </c>
@@ -3131,8 +3404,11 @@
       <c r="F107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B108" t="s">
         <v>237</v>
       </c>
@@ -3148,8 +3424,11 @@
       <c r="F108">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B109" t="s">
         <v>238</v>
       </c>
@@ -3165,8 +3444,11 @@
       <c r="F109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B110" t="s">
         <v>239</v>
       </c>
@@ -3182,8 +3464,11 @@
       <c r="F110">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="4:6" x14ac:dyDescent="0.4">
+      <c r="G110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="4:7" x14ac:dyDescent="0.4">
       <c r="D114" t="s">
         <v>282</v>
       </c>
@@ -3195,8 +3480,12 @@
         <f>F116/F115 * 100</f>
         <v>92.222222222222229</v>
       </c>
-    </row>
-    <row r="115" spans="4:6" x14ac:dyDescent="0.4">
+      <c r="G114">
+        <f>G116/G115 * 100</f>
+        <v>95.6989247311828</v>
+      </c>
+    </row>
+    <row r="115" spans="4:7" x14ac:dyDescent="0.4">
       <c r="D115" t="s">
         <v>284</v>
       </c>
@@ -3208,8 +3497,12 @@
         <f xml:space="preserve"> COUNTA(F3:F110)</f>
         <v>90</v>
       </c>
-    </row>
-    <row r="116" spans="4:6" x14ac:dyDescent="0.4">
+      <c r="G115">
+        <f xml:space="preserve"> COUNTA(G3:G110)</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="116" spans="4:7" x14ac:dyDescent="0.4">
       <c r="D116" t="s">
         <v>283</v>
       </c>
@@ -3220,6 +3513,10 @@
       <c r="F116">
         <f>COUNTIF(F3:F110,"=1")</f>
         <v>83</v>
+      </c>
+      <c r="G116">
+        <f>COUNTIF(G3:G110,"=1")</f>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>